<commit_message>
Feat: add topics, update pay charts
</commit_message>
<xml_diff>
--- a/Money/Executive_English_Now/Pay_Calendar.xlsx
+++ b/Money/Executive_English_Now/Pay_Calendar.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
   <si>
     <t>Notes:</t>
   </si>
@@ -91,13 +91,38 @@
   <si>
     <t>Intermediate Class, David &amp; Mario, +1, No Show, Rodrigo</t>
   </si>
+  <si>
+    <t>Intermediate Class, Jaime, Mario &amp; David, +2</t>
+  </si>
+  <si>
+    <t>Advance Class, Jaime, Rodrigo,  +2</t>
+  </si>
+  <si>
+    <t>Intermediate Class, Carol, Mario &amp; David, +2</t>
+  </si>
+  <si>
+    <t>Intermediate Class, Mario &amp; David, +3</t>
+  </si>
+  <si>
+    <t>Hours:</t>
+  </si>
+  <si>
+    <t>Total Hours:</t>
+  </si>
+  <si>
+    <t>Subtotal Salary:</t>
+  </si>
+  <si>
+    <t>Salary Subtotal:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd"/>
+    <numFmt numFmtId="165" formatCode="[$$-340A]#,##0.00"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -383,7 +408,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="9">
       <alignment horizontal="center"/>
@@ -429,6 +454,12 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="8">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -819,10 +850,10 @@
     <tabColor theme="4" tint="-0.249977111117893"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H168"/>
+  <dimension ref="A1:L168"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -831,10 +862,12 @@
     <col min="2" max="2" width="18.21875" customWidth="1"/>
     <col min="3" max="8" width="17.6640625" customWidth="1"/>
     <col min="9" max="9" width="2.44140625" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="4.21875" customWidth="1"/>
     <col min="14" max="14" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="2"/>
       <c r="B1" s="1">
         <f ca="1">YEAR(TODAY())</f>
@@ -849,7 +882,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="7" t="s">
         <v>1</v>
@@ -879,7 +912,7 @@
         <v>SUNDAY</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <f t="array" aca="1" ref="B3:H3" ca="1">Days+1+DATE(Calendar1Year,Calendar1MonthOption,1)-WEEKDAY(DATE(Calendar1Year,Calendar1MonthOption,1),WeekdayOption)</f>
         <v>42912</v>
@@ -909,7 +942,7 @@
         <v>42918</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -918,7 +951,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <f t="array" aca="1" ref="B5:H5" ca="1">Days+8+DATE(Calendar1Year,Calendar1MonthOption,1)-WEEKDAY(DATE(Calendar1Year,Calendar1MonthOption,1),WeekdayOption)</f>
         <v>42919</v>
@@ -948,7 +981,7 @@
         <v>42925</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -957,7 +990,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <f t="array" aca="1" ref="B7:H7" ca="1">Days+15+DATE(Calendar1Year,Calendar1MonthOption,1)-WEEKDAY(DATE(Calendar1Year,Calendar1MonthOption,1),WeekdayOption)</f>
         <v>42926</v>
@@ -986,8 +1019,14 @@
         <f ca="1"/>
         <v>42932</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>3</v>
       </c>
@@ -1006,7 +1045,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <f t="array" aca="1" ref="B9:H9" ca="1">Days+22+DATE(Calendar1Year,Calendar1MonthOption,1)-WEEKDAY(DATE(Calendar1Year,Calendar1MonthOption,1),WeekdayOption)</f>
         <v>42933</v>
@@ -1035,8 +1074,14 @@
         <f ca="1"/>
         <v>42939</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>3</v>
       </c>
@@ -1055,7 +1100,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <f t="array" aca="1" ref="B11:H11" ca="1">Days+29+DATE(Calendar1Year,Calendar1MonthOption,1)-WEEKDAY(DATE(Calendar1Year,Calendar1MonthOption,1),WeekdayOption)</f>
         <v>42940</v>
@@ -1084,8 +1129,14 @@
         <f ca="1"/>
         <v>42946</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
         <v>5</v>
       </c>
@@ -1095,12 +1146,16 @@
       <c r="D12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="G12" s="10"/>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <f t="array" aca="1" ref="B13:C13" ca="1">Days+36+DATE(Calendar1Year,Calendar1MonthOption,1)-WEEKDAY(DATE(Calendar1Year,Calendar1MonthOption,1),WeekdayOption)</f>
         <v>42947</v>
@@ -1116,8 +1171,15 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
-    </row>
-    <row r="14" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <f>SUM(K7:K12)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="13"/>
@@ -1125,8 +1187,16 @@
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="J14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="19">
+        <f>K13*15000</f>
+        <v>405000</v>
+      </c>
+      <c r="L14" s="19"/>
+    </row>
+    <row r="15" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A15" s="2"/>
       <c r="B15" s="1">
         <f ca="1">YEAR(DATE(Calendar1Year,Calendar1MonthOption+1,1))</f>
@@ -1142,7 +1212,7 @@
       <c r="G15" s="9"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="7" t="str">
         <f ca="1">UPPER(TEXT(B17,"dddd"))</f>
@@ -1173,7 +1243,7 @@
         <v>SUNDAY</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <f t="array" aca="1" ref="B17:H17" ca="1">Days+1+DATE(Calendar2Year,Calendar2MonthOption,1)-WEEKDAY(DATE(Calendar2Year,Calendar2MonthOption,1),WeekdayOption)</f>
         <v>42947</v>
@@ -1202,17 +1272,33 @@
         <f ca="1"/>
         <v>42953</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="J17" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="G18" s="10"/>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <f t="array" aca="1" ref="B19:H19" ca="1">Days+8+DATE(Calendar2Year,Calendar2MonthOption,1)-WEEKDAY(DATE(Calendar2Year,Calendar2MonthOption,1),WeekdayOption)</f>
         <v>42954</v>
@@ -1241,8 +1327,11 @@
         <f ca="1"/>
         <v>42960</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1251,7 +1340,7 @@
       <c r="G20" s="10"/>
       <c r="H20" s="11"/>
     </row>
-    <row r="21" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4">
         <f t="array" aca="1" ref="B21:H21" ca="1">Days+15+DATE(Calendar2Year,Calendar2MonthOption,1)-WEEKDAY(DATE(Calendar2Year,Calendar2MonthOption,1),WeekdayOption)</f>
         <v>42961</v>
@@ -1280,8 +1369,11 @@
         <f ca="1"/>
         <v>42967</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1290,7 +1382,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="11"/>
     </row>
-    <row r="23" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
         <f t="array" aca="1" ref="B23:H23" ca="1">Days+22+DATE(Calendar2Year,Calendar2MonthOption,1)-WEEKDAY(DATE(Calendar2Year,Calendar2MonthOption,1),WeekdayOption)</f>
         <v>42968</v>
@@ -1319,8 +1411,11 @@
         <f ca="1"/>
         <v>42974</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -1329,7 +1424,7 @@
       <c r="G24" s="10"/>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <f t="array" aca="1" ref="B25:H25" ca="1">Days+29+DATE(Calendar2Year,Calendar2MonthOption,1)-WEEKDAY(DATE(Calendar2Year,Calendar2MonthOption,1),WeekdayOption)</f>
         <v>42975</v>
@@ -1358,8 +1453,11 @@
         <f ca="1"/>
         <v>42981</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -1368,7 +1466,7 @@
       <c r="G26" s="10"/>
       <c r="H26" s="12"/>
     </row>
-    <row r="27" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
         <f t="array" aca="1" ref="B27:C27" ca="1">Days+36+DATE(Calendar2Year,Calendar2MonthOption,1)-WEEKDAY(DATE(Calendar2Year,Calendar2MonthOption,1),WeekdayOption)</f>
         <v>42982</v>
@@ -1384,8 +1482,15 @@
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
-    </row>
-    <row r="28" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J27" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27">
+        <f>SUM(K17:K26)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="13"/>
@@ -1393,8 +1498,16 @@
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
-    </row>
-    <row r="29" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="J28" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K28" s="19">
+        <f>K27*15000</f>
+        <v>255000</v>
+      </c>
+      <c r="L28" s="19"/>
+    </row>
+    <row r="29" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A29" s="2"/>
       <c r="B29" s="1">
         <f ca="1">YEAR(DATE(Calendar2Year,Calendar2MonthOption+1,1))</f>
@@ -1410,7 +1523,7 @@
       <c r="G29" s="9"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="7" t="str">
         <f ca="1">UPPER(TEXT(B31,"dddd"))</f>
@@ -1441,7 +1554,7 @@
         <v>SUNDAY</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4">
         <f t="array" aca="1" ref="B31:H31" ca="1">Days+1+DATE(Calendar3Year,Calendar3MonthOption,1)-WEEKDAY(DATE(Calendar3Year,Calendar3MonthOption,1),WeekdayOption)</f>
         <v>42975</v>
@@ -1471,7 +1584,7 @@
         <v>42981</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -4071,7 +4184,9 @@
       <c r="H168" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="26">
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K28:L28"/>
     <mergeCell ref="D83:H83"/>
     <mergeCell ref="D153:H153"/>
     <mergeCell ref="D13:H13"/>

</xml_diff>

<commit_message>
Chore: Update pay charts
</commit_message>
<xml_diff>
--- a/Money/Executive_English_Now/Pay_Calendar.xlsx
+++ b/Money/Executive_English_Now/Pay_Calendar.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
   <si>
     <t>Notes:</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Salary Subtotal:</t>
+  </si>
+  <si>
+    <t>Advance Class, Rodrigo, +3</t>
   </si>
 </sst>
 </file>
@@ -440,8 +443,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="6" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="8" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -452,14 +458,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="8">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -852,8 +855,8 @@
   </sheetPr>
   <dimension ref="A1:L168"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,13 +1167,13 @@
         <f ca="1"/>
         <v>42948</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
       <c r="J13" t="s">
         <v>12</v>
       </c>
@@ -1182,19 +1185,19 @@
     <row r="14" spans="1:12" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="J14" s="18" t="s">
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="J14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="14">
         <f>K13*15000</f>
         <v>405000</v>
       </c>
-      <c r="L14" s="19"/>
+      <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A15" s="2"/>
@@ -1332,8 +1335,12 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+      <c r="B20" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -1475,13 +1482,13 @@
         <f ca="1"/>
         <v>42983</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
       <c r="J27" t="s">
         <v>12</v>
       </c>
@@ -1493,19 +1500,19 @@
     <row r="28" spans="1:12" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="J28" s="18" t="s">
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="J28" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="19">
+      <c r="K28" s="14">
         <f>K27*15000</f>
         <v>255000</v>
       </c>
-      <c r="L28" s="19"/>
+      <c r="L28" s="14"/>
     </row>
     <row r="29" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A29" s="2"/>
@@ -1758,22 +1765,22 @@
         <f ca="1"/>
         <v>43011</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
     </row>
     <row r="42" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
     </row>
     <row r="43" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A43" s="2"/>
@@ -2026,22 +2033,22 @@
         <f ca="1"/>
         <v>43039</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
     </row>
     <row r="56" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
     </row>
     <row r="57" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A57" s="2"/>
@@ -2294,22 +2301,22 @@
         <f ca="1"/>
         <v>43074</v>
       </c>
-      <c r="D69" s="14" t="s">
+      <c r="D69" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
     </row>
     <row r="70" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
     </row>
     <row r="71" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A71" s="2"/>
@@ -2562,22 +2569,22 @@
         <f ca="1"/>
         <v>43102</v>
       </c>
-      <c r="D83" s="14" t="s">
+      <c r="D83" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E83" s="15"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="15"/>
-      <c r="H83" s="15"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="16"/>
     </row>
     <row r="84" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
     </row>
     <row r="85" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A85" s="2"/>
@@ -2830,22 +2837,22 @@
         <f ca="1"/>
         <v>43137</v>
       </c>
-      <c r="D97" s="14" t="s">
+      <c r="D97" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="15"/>
-      <c r="F97" s="15"/>
-      <c r="G97" s="15"/>
-      <c r="H97" s="15"/>
+      <c r="E97" s="16"/>
+      <c r="F97" s="16"/>
+      <c r="G97" s="16"/>
+      <c r="H97" s="16"/>
     </row>
     <row r="98" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="18"/>
     </row>
     <row r="99" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A99" s="2"/>
@@ -3098,22 +3105,22 @@
         <f ca="1"/>
         <v>43165</v>
       </c>
-      <c r="D111" s="14" t="s">
+      <c r="D111" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E111" s="15"/>
-      <c r="F111" s="15"/>
-      <c r="G111" s="15"/>
-      <c r="H111" s="15"/>
+      <c r="E111" s="16"/>
+      <c r="F111" s="16"/>
+      <c r="G111" s="16"/>
+      <c r="H111" s="16"/>
     </row>
     <row r="112" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
-      <c r="D112" s="13"/>
-      <c r="E112" s="13"/>
-      <c r="F112" s="13"/>
-      <c r="G112" s="13"/>
-      <c r="H112" s="13"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="18"/>
+      <c r="H112" s="18"/>
     </row>
     <row r="113" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A113" s="2"/>
@@ -3366,22 +3373,22 @@
         <f ca="1"/>
         <v>43193</v>
       </c>
-      <c r="D125" s="14" t="s">
+      <c r="D125" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E125" s="15"/>
-      <c r="F125" s="15"/>
-      <c r="G125" s="15"/>
-      <c r="H125" s="15"/>
+      <c r="E125" s="16"/>
+      <c r="F125" s="16"/>
+      <c r="G125" s="16"/>
+      <c r="H125" s="16"/>
     </row>
     <row r="126" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="10"/>
       <c r="C126" s="10"/>
-      <c r="D126" s="13"/>
-      <c r="E126" s="13"/>
-      <c r="F126" s="13"/>
-      <c r="G126" s="13"/>
-      <c r="H126" s="13"/>
+      <c r="D126" s="18"/>
+      <c r="E126" s="18"/>
+      <c r="F126" s="18"/>
+      <c r="G126" s="18"/>
+      <c r="H126" s="18"/>
     </row>
     <row r="127" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A127" s="2"/>
@@ -3634,22 +3641,22 @@
         <f ca="1"/>
         <v>43221</v>
       </c>
-      <c r="D139" s="14" t="s">
+      <c r="D139" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E139" s="15"/>
-      <c r="F139" s="15"/>
-      <c r="G139" s="15"/>
-      <c r="H139" s="15"/>
+      <c r="E139" s="16"/>
+      <c r="F139" s="16"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="16"/>
     </row>
     <row r="140" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
-      <c r="D140" s="13"/>
-      <c r="E140" s="13"/>
-      <c r="F140" s="13"/>
-      <c r="G140" s="13"/>
-      <c r="H140" s="13"/>
+      <c r="D140" s="18"/>
+      <c r="E140" s="18"/>
+      <c r="F140" s="18"/>
+      <c r="G140" s="18"/>
+      <c r="H140" s="18"/>
     </row>
     <row r="141" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B141" s="1">
@@ -3900,22 +3907,22 @@
         <f ca="1"/>
         <v>43256</v>
       </c>
-      <c r="D153" s="14" t="s">
+      <c r="D153" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E153" s="15"/>
-      <c r="F153" s="15"/>
-      <c r="G153" s="15"/>
-      <c r="H153" s="15"/>
+      <c r="E153" s="16"/>
+      <c r="F153" s="16"/>
+      <c r="G153" s="16"/>
+      <c r="H153" s="16"/>
     </row>
     <row r="154" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="10"/>
       <c r="C154" s="10"/>
-      <c r="D154" s="13"/>
-      <c r="E154" s="13"/>
-      <c r="F154" s="13"/>
-      <c r="G154" s="13"/>
-      <c r="H154" s="13"/>
+      <c r="D154" s="18"/>
+      <c r="E154" s="18"/>
+      <c r="F154" s="18"/>
+      <c r="G154" s="18"/>
+      <c r="H154" s="18"/>
     </row>
     <row r="155" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B155" s="1">
@@ -4166,25 +4173,37 @@
         <f ca="1"/>
         <v>43284</v>
       </c>
-      <c r="D167" s="14" t="s">
+      <c r="D167" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E167" s="15"/>
-      <c r="F167" s="15"/>
-      <c r="G167" s="15"/>
-      <c r="H167" s="15"/>
+      <c r="E167" s="16"/>
+      <c r="F167" s="16"/>
+      <c r="G167" s="16"/>
+      <c r="H167" s="16"/>
     </row>
     <row r="168" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="10"/>
       <c r="C168" s="10"/>
-      <c r="D168" s="13"/>
-      <c r="E168" s="13"/>
-      <c r="F168" s="13"/>
-      <c r="G168" s="13"/>
-      <c r="H168" s="13"/>
+      <c r="D168" s="18"/>
+      <c r="E168" s="18"/>
+      <c r="F168" s="18"/>
+      <c r="G168" s="18"/>
+      <c r="H168" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D168:H168"/>
+    <mergeCell ref="D139:H139"/>
+    <mergeCell ref="D140:H140"/>
+    <mergeCell ref="D97:H97"/>
+    <mergeCell ref="D84:H84"/>
+    <mergeCell ref="D126:H126"/>
+    <mergeCell ref="D111:H111"/>
+    <mergeCell ref="D125:H125"/>
+    <mergeCell ref="D98:H98"/>
+    <mergeCell ref="D112:H112"/>
+    <mergeCell ref="D154:H154"/>
+    <mergeCell ref="D167:H167"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="D83:H83"/>
@@ -4199,18 +4218,6 @@
     <mergeCell ref="D27:H27"/>
     <mergeCell ref="D28:H28"/>
     <mergeCell ref="D41:H41"/>
-    <mergeCell ref="D168:H168"/>
-    <mergeCell ref="D139:H139"/>
-    <mergeCell ref="D140:H140"/>
-    <mergeCell ref="D97:H97"/>
-    <mergeCell ref="D84:H84"/>
-    <mergeCell ref="D126:H126"/>
-    <mergeCell ref="D111:H111"/>
-    <mergeCell ref="D125:H125"/>
-    <mergeCell ref="D98:H98"/>
-    <mergeCell ref="D112:H112"/>
-    <mergeCell ref="D154:H154"/>
-    <mergeCell ref="D167:H167"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:H3 B5:H5 B7:H7 B9:H9 B11:H11 B13:C13">

</xml_diff>

<commit_message>
Feat: Add calanders for Maria and Claudio
</commit_message>
<xml_diff>
--- a/Money/Executive_English_Now/Pay_Calendar.xlsx
+++ b/Money/Executive_English_Now/Pay_Calendar.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>Notes:</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>Advanced/Intermediate, Mario &amp; David, Jaime, +2</t>
+  </si>
+  <si>
+    <t>Intermediate Class, Mario &amp; David, Jamie, +2</t>
+  </si>
+  <si>
+    <t>Advance Class, Jaime, +3</t>
   </si>
 </sst>
 </file>
@@ -452,8 +458,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="8" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -461,11 +467,11 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="8" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="8">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -861,8 +867,8 @@
   </sheetPr>
   <dimension ref="A1:M168"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1173,13 +1179,13 @@
         <f ca="1"/>
         <v>42948</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
       <c r="J13" t="s">
         <v>12</v>
       </c>
@@ -1191,19 +1197,19 @@
     <row r="14" spans="1:12" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
       <c r="J14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="14">
         <f>K13*15000</f>
         <v>405000</v>
       </c>
-      <c r="L14" s="17"/>
+      <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A15" s="2"/>
@@ -1394,13 +1400,22 @@
       <c r="J21" t="s">
         <v>11</v>
       </c>
+      <c r="K21">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="1:13" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="G22" s="10"/>
       <c r="H22" s="11"/>
     </row>
@@ -1436,10 +1451,17 @@
       <c r="J23" t="s">
         <v>11</v>
       </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:13" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
+      <c r="B24" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -1509,26 +1531,26 @@
       </c>
       <c r="K27">
         <f>SUM(K17:K26)</f>
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
       <c r="J28" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="17">
+      <c r="K28" s="14">
         <f>K27*15000</f>
-        <v>510000</v>
-      </c>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
+        <v>765000</v>
+      </c>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
     </row>
     <row r="29" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A29" s="2"/>
@@ -1792,11 +1814,11 @@
     <row r="42" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
     </row>
     <row r="43" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A43" s="2"/>
@@ -2060,11 +2082,11 @@
     <row r="56" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
     </row>
     <row r="57" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A57" s="2"/>
@@ -2328,11 +2350,11 @@
     <row r="70" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
     </row>
     <row r="71" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A71" s="2"/>
@@ -2596,11 +2618,11 @@
     <row r="84" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
     </row>
     <row r="85" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A85" s="2"/>
@@ -2864,11 +2886,11 @@
     <row r="98" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
-      <c r="D98" s="14"/>
-      <c r="E98" s="14"/>
-      <c r="F98" s="14"/>
-      <c r="G98" s="14"/>
-      <c r="H98" s="14"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="18"/>
     </row>
     <row r="99" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A99" s="2"/>
@@ -3132,11 +3154,11 @@
     <row r="112" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
-      <c r="D112" s="14"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="14"/>
-      <c r="G112" s="14"/>
-      <c r="H112" s="14"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="18"/>
+      <c r="H112" s="18"/>
     </row>
     <row r="113" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A113" s="2"/>
@@ -3400,11 +3422,11 @@
     <row r="126" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="10"/>
       <c r="C126" s="10"/>
-      <c r="D126" s="14"/>
-      <c r="E126" s="14"/>
-      <c r="F126" s="14"/>
-      <c r="G126" s="14"/>
-      <c r="H126" s="14"/>
+      <c r="D126" s="18"/>
+      <c r="E126" s="18"/>
+      <c r="F126" s="18"/>
+      <c r="G126" s="18"/>
+      <c r="H126" s="18"/>
     </row>
     <row r="127" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A127" s="2"/>
@@ -3668,11 +3690,11 @@
     <row r="140" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
-      <c r="D140" s="14"/>
-      <c r="E140" s="14"/>
-      <c r="F140" s="14"/>
-      <c r="G140" s="14"/>
-      <c r="H140" s="14"/>
+      <c r="D140" s="18"/>
+      <c r="E140" s="18"/>
+      <c r="F140" s="18"/>
+      <c r="G140" s="18"/>
+      <c r="H140" s="18"/>
     </row>
     <row r="141" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B141" s="1">
@@ -3934,11 +3956,11 @@
     <row r="154" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="10"/>
       <c r="C154" s="10"/>
-      <c r="D154" s="14"/>
-      <c r="E154" s="14"/>
-      <c r="F154" s="14"/>
-      <c r="G154" s="14"/>
-      <c r="H154" s="14"/>
+      <c r="D154" s="18"/>
+      <c r="E154" s="18"/>
+      <c r="F154" s="18"/>
+      <c r="G154" s="18"/>
+      <c r="H154" s="18"/>
     </row>
     <row r="155" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B155" s="1">
@@ -4200,14 +4222,26 @@
     <row r="168" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="10"/>
       <c r="C168" s="10"/>
-      <c r="D168" s="14"/>
-      <c r="E168" s="14"/>
-      <c r="F168" s="14"/>
-      <c r="G168" s="14"/>
-      <c r="H168" s="14"/>
+      <c r="D168" s="18"/>
+      <c r="E168" s="18"/>
+      <c r="F168" s="18"/>
+      <c r="G168" s="18"/>
+      <c r="H168" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D168:H168"/>
+    <mergeCell ref="D139:H139"/>
+    <mergeCell ref="D140:H140"/>
+    <mergeCell ref="D97:H97"/>
+    <mergeCell ref="D84:H84"/>
+    <mergeCell ref="D126:H126"/>
+    <mergeCell ref="D111:H111"/>
+    <mergeCell ref="D125:H125"/>
+    <mergeCell ref="D98:H98"/>
+    <mergeCell ref="D112:H112"/>
+    <mergeCell ref="D154:H154"/>
+    <mergeCell ref="D167:H167"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="D83:H83"/>
     <mergeCell ref="D153:H153"/>
@@ -4222,18 +4256,6 @@
     <mergeCell ref="D28:H28"/>
     <mergeCell ref="D41:H41"/>
     <mergeCell ref="K28:M28"/>
-    <mergeCell ref="D168:H168"/>
-    <mergeCell ref="D139:H139"/>
-    <mergeCell ref="D140:H140"/>
-    <mergeCell ref="D97:H97"/>
-    <mergeCell ref="D84:H84"/>
-    <mergeCell ref="D126:H126"/>
-    <mergeCell ref="D111:H111"/>
-    <mergeCell ref="D125:H125"/>
-    <mergeCell ref="D98:H98"/>
-    <mergeCell ref="D112:H112"/>
-    <mergeCell ref="D154:H154"/>
-    <mergeCell ref="D167:H167"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:H3 B5:H5 B7:H7 B9:H9 B11:H11 B13:C13">

</xml_diff>

<commit_message>
Feat: Add calander for Antonio
</commit_message>
<xml_diff>
--- a/Money/Executive_English_Now/Pay_Calendar.xlsx
+++ b/Money/Executive_English_Now/Pay_Calendar.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
   <si>
     <t>Notes:</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Advanced Class</t>
   </si>
 </sst>
 </file>
@@ -470,8 +473,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="8" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -479,11 +482,11 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="8" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="8">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -879,8 +882,8 @@
   </sheetPr>
   <dimension ref="A1:O168"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1191,13 +1194,13 @@
         <f ca="1"/>
         <v>42948</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
       <c r="J13" t="s">
         <v>12</v>
       </c>
@@ -1209,19 +1212,19 @@
     <row r="14" spans="1:15" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
       <c r="J14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="14">
         <f>K13*15000</f>
         <v>405000</v>
       </c>
-      <c r="L14" s="17"/>
+      <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A15" s="2"/>
@@ -1380,7 +1383,7 @@
         <v>12</v>
       </c>
       <c r="O19">
-        <f t="shared" ref="O19:O26" si="2">K19+M19</f>
+        <f t="shared" ref="O19" si="2">K19+M19</f>
         <v>17</v>
       </c>
     </row>
@@ -1442,7 +1445,7 @@
         <v>4</v>
       </c>
       <c r="O21">
-        <f t="shared" ref="O21:O26" si="3">K21+M21</f>
+        <f t="shared" ref="O21" si="3">K21+M21</f>
         <v>7</v>
       </c>
     </row>
@@ -1500,7 +1503,7 @@
         <v>10</v>
       </c>
       <c r="O23">
-        <f t="shared" ref="O23:O26" si="4">K23+M23</f>
+        <f t="shared" ref="O23" si="4">K23+M23</f>
         <v>15</v>
       </c>
     </row>
@@ -1556,18 +1559,26 @@
         <v>11</v>
       </c>
       <c r="K25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O25">
-        <f t="shared" ref="O25:O26" si="5">K25+M25</f>
-        <v>5</v>
+        <f t="shared" ref="O25" si="5">K25+M25</f>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
+      <c r="B26" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="12"/>
@@ -1593,34 +1604,34 @@
       </c>
       <c r="K27">
         <f>SUM(K17:K26)</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M27">
-        <f t="shared" ref="L27:O27" si="6">SUM(M17:M26)</f>
+        <f t="shared" ref="M27:O27" si="6">SUM(M17:M26)</f>
         <v>38</v>
       </c>
       <c r="O27">
         <f t="shared" si="6"/>
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
       <c r="J28" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="17">
+      <c r="K28" s="14">
         <f>O27*15000</f>
-        <v>915000</v>
-      </c>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
+        <v>900000</v>
+      </c>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
     </row>
     <row r="29" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A29" s="2"/>
@@ -1884,11 +1895,11 @@
     <row r="42" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
     </row>
     <row r="43" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A43" s="2"/>
@@ -2152,11 +2163,11 @@
     <row r="56" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
     </row>
     <row r="57" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A57" s="2"/>
@@ -2420,11 +2431,11 @@
     <row r="70" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
     </row>
     <row r="71" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A71" s="2"/>
@@ -2688,11 +2699,11 @@
     <row r="84" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
     </row>
     <row r="85" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A85" s="2"/>
@@ -2956,11 +2967,11 @@
     <row r="98" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
-      <c r="D98" s="14"/>
-      <c r="E98" s="14"/>
-      <c r="F98" s="14"/>
-      <c r="G98" s="14"/>
-      <c r="H98" s="14"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="18"/>
     </row>
     <row r="99" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A99" s="2"/>
@@ -3224,11 +3235,11 @@
     <row r="112" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
-      <c r="D112" s="14"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="14"/>
-      <c r="G112" s="14"/>
-      <c r="H112" s="14"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="18"/>
+      <c r="H112" s="18"/>
     </row>
     <row r="113" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A113" s="2"/>
@@ -3492,11 +3503,11 @@
     <row r="126" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="10"/>
       <c r="C126" s="10"/>
-      <c r="D126" s="14"/>
-      <c r="E126" s="14"/>
-      <c r="F126" s="14"/>
-      <c r="G126" s="14"/>
-      <c r="H126" s="14"/>
+      <c r="D126" s="18"/>
+      <c r="E126" s="18"/>
+      <c r="F126" s="18"/>
+      <c r="G126" s="18"/>
+      <c r="H126" s="18"/>
     </row>
     <row r="127" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A127" s="2"/>
@@ -3760,11 +3771,11 @@
     <row r="140" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
-      <c r="D140" s="14"/>
-      <c r="E140" s="14"/>
-      <c r="F140" s="14"/>
-      <c r="G140" s="14"/>
-      <c r="H140" s="14"/>
+      <c r="D140" s="18"/>
+      <c r="E140" s="18"/>
+      <c r="F140" s="18"/>
+      <c r="G140" s="18"/>
+      <c r="H140" s="18"/>
     </row>
     <row r="141" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B141" s="1">
@@ -4026,11 +4037,11 @@
     <row r="154" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="10"/>
       <c r="C154" s="10"/>
-      <c r="D154" s="14"/>
-      <c r="E154" s="14"/>
-      <c r="F154" s="14"/>
-      <c r="G154" s="14"/>
-      <c r="H154" s="14"/>
+      <c r="D154" s="18"/>
+      <c r="E154" s="18"/>
+      <c r="F154" s="18"/>
+      <c r="G154" s="18"/>
+      <c r="H154" s="18"/>
     </row>
     <row r="155" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B155" s="1">
@@ -4292,14 +4303,26 @@
     <row r="168" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="10"/>
       <c r="C168" s="10"/>
-      <c r="D168" s="14"/>
-      <c r="E168" s="14"/>
-      <c r="F168" s="14"/>
-      <c r="G168" s="14"/>
-      <c r="H168" s="14"/>
+      <c r="D168" s="18"/>
+      <c r="E168" s="18"/>
+      <c r="F168" s="18"/>
+      <c r="G168" s="18"/>
+      <c r="H168" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D168:H168"/>
+    <mergeCell ref="D139:H139"/>
+    <mergeCell ref="D140:H140"/>
+    <mergeCell ref="D97:H97"/>
+    <mergeCell ref="D84:H84"/>
+    <mergeCell ref="D126:H126"/>
+    <mergeCell ref="D111:H111"/>
+    <mergeCell ref="D125:H125"/>
+    <mergeCell ref="D98:H98"/>
+    <mergeCell ref="D112:H112"/>
+    <mergeCell ref="D154:H154"/>
+    <mergeCell ref="D167:H167"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="D83:H83"/>
     <mergeCell ref="D153:H153"/>
@@ -4314,18 +4337,6 @@
     <mergeCell ref="D28:H28"/>
     <mergeCell ref="D41:H41"/>
     <mergeCell ref="K28:M28"/>
-    <mergeCell ref="D168:H168"/>
-    <mergeCell ref="D139:H139"/>
-    <mergeCell ref="D140:H140"/>
-    <mergeCell ref="D97:H97"/>
-    <mergeCell ref="D84:H84"/>
-    <mergeCell ref="D126:H126"/>
-    <mergeCell ref="D111:H111"/>
-    <mergeCell ref="D125:H125"/>
-    <mergeCell ref="D98:H98"/>
-    <mergeCell ref="D112:H112"/>
-    <mergeCell ref="D154:H154"/>
-    <mergeCell ref="D167:H167"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:H3 B5:H5 B7:H7 B9:H9 B11:H11 B13:C13">

</xml_diff>